<commit_message>
Added total body fat variable
</commit_message>
<xml_diff>
--- a/data/CKM Variable List.xlsx
+++ b/data/CKM Variable List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\nhanes_ckm\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishnasanaka/nhanes_ckm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A0DE2D-628E-482A-AE61-BB43EA644ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FCD678-28CA-C241-9E5F-B5C2AE0A307E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-15840" windowWidth="16440" windowHeight="28440" firstSheet="12" activeTab="12" xr2:uid="{9B035D0F-8A45-D344-8416-9889809E00CA}"/>
+    <workbookView xWindow="4800" yWindow="500" windowWidth="28800" windowHeight="15780" firstSheet="6" activeTab="11" xr2:uid="{9B035D0F-8A45-D344-8416-9889809E00CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="26" r:id="rId1"/>
@@ -23,23 +23,24 @@
     <sheet name="CDQ" sheetId="7" r:id="rId8"/>
     <sheet name="DEMO" sheetId="8" r:id="rId9"/>
     <sheet name="DIQ" sheetId="9" r:id="rId10"/>
-    <sheet name="FASTQX" sheetId="27" r:id="rId11"/>
-    <sheet name="GHB" sheetId="10" r:id="rId12"/>
-    <sheet name="GLU" sheetId="11" r:id="rId13"/>
-    <sheet name="HDL" sheetId="12" r:id="rId14"/>
-    <sheet name="HSCRP" sheetId="13" r:id="rId15"/>
-    <sheet name="HUQ" sheetId="14" r:id="rId16"/>
-    <sheet name="INQ" sheetId="15" r:id="rId17"/>
-    <sheet name="INS" sheetId="16" r:id="rId18"/>
-    <sheet name="KIQ_U" sheetId="17" r:id="rId19"/>
-    <sheet name="MCQ" sheetId="18" r:id="rId20"/>
-    <sheet name="OGTT" sheetId="25" r:id="rId21"/>
-    <sheet name="RXQASA" sheetId="19" r:id="rId22"/>
-    <sheet name="SMQ" sheetId="20" r:id="rId23"/>
-    <sheet name="SMQRTU" sheetId="21" r:id="rId24"/>
-    <sheet name="SSAGP" sheetId="22" r:id="rId25"/>
-    <sheet name="TCHOL" sheetId="23" r:id="rId26"/>
-    <sheet name="TRIGLY" sheetId="24" r:id="rId27"/>
+    <sheet name="DXX" sheetId="30" r:id="rId11"/>
+    <sheet name="FASTQX" sheetId="27" r:id="rId12"/>
+    <sheet name="GHB" sheetId="10" r:id="rId13"/>
+    <sheet name="GLU" sheetId="11" r:id="rId14"/>
+    <sheet name="HDL" sheetId="12" r:id="rId15"/>
+    <sheet name="HSCRP" sheetId="13" r:id="rId16"/>
+    <sheet name="HUQ" sheetId="14" r:id="rId17"/>
+    <sheet name="INQ" sheetId="15" r:id="rId18"/>
+    <sheet name="INS" sheetId="16" r:id="rId19"/>
+    <sheet name="KIQ_U" sheetId="17" r:id="rId20"/>
+    <sheet name="MCQ" sheetId="18" r:id="rId21"/>
+    <sheet name="OGTT" sheetId="25" r:id="rId22"/>
+    <sheet name="RXQASA" sheetId="19" r:id="rId23"/>
+    <sheet name="SMQ" sheetId="20" r:id="rId24"/>
+    <sheet name="SMQRTU" sheetId="21" r:id="rId25"/>
+    <sheet name="SSAGP" sheetId="22" r:id="rId26"/>
+    <sheet name="TCHOL" sheetId="23" r:id="rId27"/>
+    <sheet name="TRIGLY" sheetId="24" r:id="rId28"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -325,7 +326,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1625" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="230">
   <si>
     <t>variable</t>
   </si>
@@ -1009,6 +1010,12 @@
   </si>
   <si>
     <t>WTSAFPRP</t>
+  </si>
+  <si>
+    <t>total_fat</t>
+  </si>
+  <si>
+    <t>DXDTOFAT</t>
   </si>
 </sst>
 </file>
@@ -1079,13 +1086,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1542,18 +1548,18 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>216</v>
       </c>
       <c r="B2" t="s">
@@ -1563,7 +1569,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>214</v>
       </c>
@@ -1574,12 +1580,12 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>221</v>
       </c>
@@ -1594,12 +1600,12 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="L2" sqref="A2:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1637,7 +1643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1675,7 +1681,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1713,7 +1719,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1751,7 +1757,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1783,7 +1789,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -1821,7 +1827,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -1859,7 +1865,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1897,7 +1903,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>85</v>
       </c>
@@ -1935,7 +1941,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -1967,19 +1973,148 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BF2F90-C323-1349-A243-99F38CFCA105}">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" t="s">
+        <v>229</v>
+      </c>
+      <c r="F3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G3" t="s">
+        <v>229</v>
+      </c>
+      <c r="H3" t="s">
+        <v>229</v>
+      </c>
+      <c r="I3" t="s">
+        <v>229</v>
+      </c>
+      <c r="J3" t="s">
+        <v>229</v>
+      </c>
+      <c r="K3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B87265F-26C7-4386-8B52-059591A00490}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2017,7 +2152,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2055,7 +2190,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>223</v>
       </c>
@@ -2093,7 +2228,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2111,7 +2246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C29EFAD-03F0-B447-A983-4B5565025BC2}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -2119,9 +2254,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2159,7 +2294,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2197,7 +2332,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -2233,174 +2368,6 @@
       </c>
       <c r="L3" t="s">
         <v>134</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270977A7-E7B7-C047-9DBF-59746F13B1CD}">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G3" t="s">
-        <v>138</v>
-      </c>
-      <c r="H3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I3" t="s">
-        <v>138</v>
-      </c>
-      <c r="J3" t="s">
-        <v>138</v>
-      </c>
-      <c r="K3" t="s">
-        <v>138</v>
-      </c>
-      <c r="L3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>224</v>
-      </c>
-      <c r="B4" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" t="s">
-        <v>225</v>
-      </c>
-      <c r="D4" t="s">
-        <v>225</v>
-      </c>
-      <c r="E4" t="s">
-        <v>225</v>
-      </c>
-      <c r="F4" t="s">
-        <v>225</v>
-      </c>
-      <c r="G4" t="s">
-        <v>225</v>
-      </c>
-      <c r="H4" t="s">
-        <v>225</v>
-      </c>
-      <c r="I4" t="s">
-        <v>225</v>
-      </c>
-      <c r="J4" t="s">
-        <v>225</v>
-      </c>
-      <c r="K4" t="s">
-        <v>225</v>
-      </c>
-      <c r="L4" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -2410,6 +2377,174 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270977A7-E7B7-C047-9DBF-59746F13B1CD}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" t="s">
+        <v>138</v>
+      </c>
+      <c r="J3" t="s">
+        <v>138</v>
+      </c>
+      <c r="K3" t="s">
+        <v>138</v>
+      </c>
+      <c r="L3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E4" t="s">
+        <v>225</v>
+      </c>
+      <c r="F4" t="s">
+        <v>225</v>
+      </c>
+      <c r="G4" t="s">
+        <v>225</v>
+      </c>
+      <c r="H4" t="s">
+        <v>225</v>
+      </c>
+      <c r="I4" t="s">
+        <v>225</v>
+      </c>
+      <c r="J4" t="s">
+        <v>225</v>
+      </c>
+      <c r="K4" t="s">
+        <v>225</v>
+      </c>
+      <c r="L4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85252202-D3B5-A945-8429-01698367E2C9}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -2417,9 +2552,9 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2457,7 +2592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2495,7 +2630,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2539,7 +2674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C686534B-BF02-8740-9CD8-A73AF60469ED}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -2550,9 +2685,9 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2590,7 +2725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2628,7 +2763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -2672,7 +2807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC757E38-DF6E-9C47-986A-E5D523B85FF9}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -2680,9 +2815,9 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2720,7 +2855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2763,7 +2898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A8F896-8412-FD4D-A653-D930D501E3F0}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -2774,9 +2909,9 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2814,7 +2949,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2857,7 +2992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F8F56B-9E15-EF47-B5F6-D90A8D8B0453}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -2865,12 +3000,12 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2908,7 +3043,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2946,7 +3081,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -2987,170 +3122,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B22359-510C-BD4E-946F-DF74FC3CE91E}">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J3" t="s">
-        <v>91</v>
-      </c>
-      <c r="K3" t="s">
-        <v>91</v>
-      </c>
-      <c r="L3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H4" t="s">
-        <v>93</v>
-      </c>
-      <c r="I4" t="s">
-        <v>93</v>
-      </c>
-      <c r="J4" t="s">
-        <v>93</v>
-      </c>
-      <c r="K4" t="s">
-        <v>93</v>
-      </c>
-      <c r="L4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3163,13 +3134,13 @@
       <selection pane="topRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3207,7 +3178,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3245,7 +3216,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -3283,7 +3254,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -3321,7 +3292,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -3352,6 +3323,170 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B22359-510C-BD4E-946F-DF74FC3CE91E}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J4" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C695FBCA-2F20-C349-9C97-E127EC92AD35}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
@@ -3359,9 +3494,9 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3399,7 +3534,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3437,7 +3572,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -3475,7 +3610,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -3513,7 +3648,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -3551,7 +3686,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -3589,7 +3724,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -3627,7 +3762,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -3665,7 +3800,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -3703,7 +3838,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -3744,7 +3879,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>103</v>
       </c>
@@ -3782,7 +3917,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>104</v>
       </c>
@@ -3820,7 +3955,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>105</v>
       </c>
@@ -3863,7 +3998,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B443EBC9-A9ED-4996-AA7B-B560C4AE0236}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
@@ -3871,9 +4006,9 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3911,7 +4046,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3943,7 +4078,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>205</v>
       </c>
@@ -3966,7 +4101,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>202</v>
       </c>
@@ -3989,7 +4124,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>203</v>
       </c>
@@ -4009,7 +4144,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="Q11" t="s">
         <v>173</v>
       </c>
@@ -4019,7 +4154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98AD27C-16C2-BE4F-BECC-445339C348A0}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -4030,9 +4165,9 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4070,7 +4205,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4108,7 +4243,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -4146,7 +4281,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -4189,7 +4324,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF0C966-3BAC-4E46-A712-3678781F85CE}">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -4197,9 +4332,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4237,7 +4372,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4275,7 +4410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -4313,7 +4448,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -4351,7 +4486,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -4394,7 +4529,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40400EB-A076-D749-9395-73DB4F782CEE}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -4402,9 +4537,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4442,7 +4577,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4480,7 +4615,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -4523,7 +4658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1A5F4B-3A4F-C646-B6D8-2975540D552C}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -4534,9 +4669,9 @@
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4574,7 +4709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4612,7 +4747,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -4656,7 +4791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9B0605-DB41-5741-AA2A-D1CA2C98BE32}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -4664,9 +4799,9 @@
       <selection activeCell="A3" sqref="A3:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4704,7 +4839,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -4742,7 +4877,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -4786,7 +4921,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0B3097-2DFA-944C-921C-4CA3796F226E}">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -4794,9 +4929,9 @@
       <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4834,7 +4969,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -4872,7 +5007,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -4910,7 +5045,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4965,9 +5100,9 @@
       <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5005,7 +5140,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5056,9 +5191,9 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5096,7 +5231,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5134,7 +5269,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -5172,7 +5307,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -5210,7 +5345,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>143</v>
       </c>
@@ -5248,7 +5383,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -5268,7 +5403,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -5306,7 +5441,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -5344,7 +5479,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>146</v>
       </c>
@@ -5396,9 +5531,9 @@
       <selection activeCell="A3" sqref="A3:L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5436,7 +5571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5474,7 +5609,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -5512,7 +5647,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -5550,7 +5685,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -5588,7 +5723,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -5639,9 +5774,9 @@
       <selection activeCell="D5" sqref="B5:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5679,7 +5814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5717,7 +5852,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -5755,7 +5890,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -5793,7 +5928,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -5819,7 +5954,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -5857,7 +5992,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -5895,7 +6030,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -5933,7 +6068,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -5971,7 +6106,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -6023,9 +6158,9 @@
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6063,7 +6198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6101,7 +6236,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -6139,7 +6274,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -6177,7 +6312,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -6215,7 +6350,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -6250,7 +6385,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -6288,7 +6423,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -6326,7 +6461,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -6364,7 +6499,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -6412,9 +6547,9 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6452,7 +6587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6503,9 +6638,9 @@
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6543,7 +6678,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6581,7 +6716,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -6619,7 +6754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -6657,7 +6792,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -6695,7 +6830,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -6733,7 +6868,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -6771,7 +6906,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -6806,7 +6941,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -6844,7 +6979,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>211</v>
       </c>
@@ -6880,7 +7015,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -6918,7 +7053,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -6956,7 +7091,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -6994,7 +7129,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -7032,7 +7167,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -7070,7 +7205,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>209</v>
       </c>
@@ -7108,7 +7243,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>208</v>
       </c>
@@ -7128,7 +7263,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Added newly diagnosed diabetes subset
</commit_message>
<xml_diff>
--- a/data/CKM Variable List.xlsx
+++ b/data/CKM Variable List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishnasanaka/nhanes_ckm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FCD678-28CA-C241-9E5F-B5C2AE0A307E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238962B2-D2A2-C749-8C67-0E095E43628B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="500" windowWidth="28800" windowHeight="15780" firstSheet="6" activeTab="11" xr2:uid="{9B035D0F-8A45-D344-8416-9889809E00CA}"/>
+    <workbookView xWindow="3680" yWindow="500" windowWidth="28800" windowHeight="15780" firstSheet="8" activeTab="23" xr2:uid="{9B035D0F-8A45-D344-8416-9889809E00CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="26" r:id="rId1"/>
@@ -326,7 +326,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1661" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="233">
   <si>
     <t>variable</t>
   </si>
@@ -1016,13 +1016,22 @@
   </si>
   <si>
     <t>DXDTOFAT</t>
+  </si>
+  <si>
+    <t>2021-2023</t>
+  </si>
+  <si>
+    <t>BPQ150</t>
+  </si>
+  <si>
+    <t>BPQ101D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1065,6 +1074,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1086,12 +1102,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1597,15 +1614,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6929FDCF-EFFB-654F-B597-6A4AD8F87EA2}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="A2:L2"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1642,8 +1659,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1680,8 +1700,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1718,8 +1741,11 @@
       <c r="L3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1756,8 +1782,11 @@
       <c r="L4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1788,8 +1817,11 @@
       <c r="L5" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -1826,8 +1858,11 @@
       <c r="L6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -1864,8 +1899,11 @@
       <c r="L7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1902,8 +1940,11 @@
       <c r="L8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>85</v>
       </c>
@@ -1940,8 +1981,11 @@
       <c r="L9" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -1974,15 +2018,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BF2F90-C323-1349-A243-99F38CFCA105}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2019,8 +2063,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2057,8 +2104,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>228</v>
       </c>
@@ -2093,6 +2143,9 @@
         <v>229</v>
       </c>
       <c r="L3" t="s">
+        <v>229</v>
+      </c>
+      <c r="M3" t="s">
         <v>229</v>
       </c>
     </row>
@@ -2103,10 +2156,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B87265F-26C7-4386-8B52-059591A00490}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2114,7 +2167,7 @@
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2151,8 +2204,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2189,8 +2245,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>223</v>
       </c>
@@ -2227,8 +2286,11 @@
       <c r="L3" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2248,15 +2310,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C29EFAD-03F0-B447-A983-4B5565025BC2}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L2" sqref="L2:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2293,8 +2355,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2331,8 +2396,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -2367,6 +2435,9 @@
         <v>134</v>
       </c>
       <c r="L3" t="s">
+        <v>134</v>
+      </c>
+      <c r="M3" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2378,15 +2449,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270977A7-E7B7-C047-9DBF-59746F13B1CD}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2423,8 +2494,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2461,8 +2535,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -2499,8 +2576,11 @@
       <c r="L3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>224</v>
       </c>
@@ -2536,6 +2616,9 @@
       </c>
       <c r="L4" t="s">
         <v>227</v>
+      </c>
+      <c r="M4" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2546,15 +2629,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85252202-D3B5-A945-8429-01698367E2C9}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2591,8 +2674,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2629,8 +2715,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2665,6 +2754,9 @@
         <v>128</v>
       </c>
       <c r="L3" t="s">
+        <v>128</v>
+      </c>
+      <c r="M3" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2679,15 +2771,15 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="L2" sqref="L2:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2724,8 +2816,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2762,8 +2857,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -2798,6 +2896,9 @@
         <v>136</v>
       </c>
       <c r="L3" t="s">
+        <v>136</v>
+      </c>
+      <c r="M3" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2809,15 +2910,15 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC757E38-DF6E-9C47-986A-E5D523B85FF9}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="L2" sqref="L2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2854,8 +2955,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2890,6 +2994,9 @@
         <v>21</v>
       </c>
       <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2903,15 +3010,15 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="L2" sqref="L2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2948,8 +3055,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2984,6 +3094,9 @@
         <v>21</v>
       </c>
       <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2994,10 +3107,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F8F56B-9E15-EF47-B5F6-D90A8D8B0453}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L2" sqref="L2:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3005,7 +3118,7 @@
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3042,8 +3155,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3080,8 +3196,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -3116,6 +3235,9 @@
         <v>140</v>
       </c>
       <c r="L3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M3" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3127,11 +3249,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B559425B-2CCE-B440-B092-DF8757C2B03D}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A21" sqref="A21"/>
+      <selection pane="topRight" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3140,7 +3262,7 @@
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3177,8 +3299,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3215,8 +3340,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -3253,8 +3381,11 @@
       <c r="L3" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -3291,8 +3422,11 @@
       <c r="L4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -3312,6 +3446,9 @@
         <v>124</v>
       </c>
       <c r="L5" t="s">
+        <v>124</v>
+      </c>
+      <c r="M5" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3324,15 +3461,15 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B22359-510C-BD4E-946F-DF74FC3CE91E}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="L2" sqref="L2:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3369,8 +3506,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3407,8 +3547,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -3445,8 +3588,11 @@
       <c r="L3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -3478,6 +3624,9 @@
         <v>93</v>
       </c>
       <c r="L4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" t="s">
         <v>93</v>
       </c>
     </row>
@@ -3491,7 +3640,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3533,6 +3682,9 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -3571,6 +3723,9 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -3647,6 +3802,9 @@
       <c r="L4" t="s">
         <v>174</v>
       </c>
+      <c r="M4" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -3723,6 +3881,9 @@
       <c r="L6" t="s">
         <v>176</v>
       </c>
+      <c r="M6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -3799,6 +3960,9 @@
       <c r="L8" t="s">
         <v>178</v>
       </c>
+      <c r="M8" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -3875,6 +4039,9 @@
       <c r="L10" t="s">
         <v>180</v>
       </c>
+      <c r="M10" t="s">
+        <v>180</v>
+      </c>
       <c r="Q10" t="s">
         <v>173</v>
       </c>
@@ -3952,6 +4119,9 @@
         <v>182</v>
       </c>
       <c r="L12" t="s">
+        <v>182</v>
+      </c>
+      <c r="M12" t="s">
         <v>182</v>
       </c>
     </row>
@@ -4003,7 +4173,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J2" sqref="J2:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4045,6 +4215,9 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -4077,6 +4250,15 @@
       <c r="J2" t="s">
         <v>21</v>
       </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -4100,6 +4282,15 @@
       <c r="J3" t="s">
         <v>206</v>
       </c>
+      <c r="K3" t="s">
+        <v>206</v>
+      </c>
+      <c r="L3" t="s">
+        <v>206</v>
+      </c>
+      <c r="M3" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -4123,6 +4314,15 @@
       <c r="J4" t="s">
         <v>204</v>
       </c>
+      <c r="K4" t="s">
+        <v>204</v>
+      </c>
+      <c r="L4" t="s">
+        <v>204</v>
+      </c>
+      <c r="M4" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -4141,6 +4341,15 @@
         <v>207</v>
       </c>
       <c r="J5" t="s">
+        <v>207</v>
+      </c>
+      <c r="K5" t="s">
+        <v>207</v>
+      </c>
+      <c r="L5" t="s">
+        <v>207</v>
+      </c>
+      <c r="M5" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4159,15 +4368,15 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4204,8 +4413,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4242,8 +4454,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -4280,8 +4495,11 @@
       <c r="L3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -4316,6 +4534,9 @@
         <v>110</v>
       </c>
       <c r="L4" t="s">
+        <v>110</v>
+      </c>
+      <c r="M4" t="s">
         <v>110</v>
       </c>
     </row>
@@ -4326,15 +4547,15 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF0C966-3BAC-4E46-A712-3678781F85CE}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4371,8 +4592,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4409,8 +4633,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -4447,8 +4674,11 @@
       <c r="L3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -4486,7 +4716,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -4521,6 +4751,9 @@
         <v>116</v>
       </c>
       <c r="L5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M5" t="s">
         <v>116</v>
       </c>
     </row>
@@ -4531,15 +4764,15 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40400EB-A076-D749-9395-73DB4F782CEE}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4576,8 +4809,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4614,8 +4850,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -4650,6 +4889,9 @@
         <v>118</v>
       </c>
       <c r="L3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M3" t="s">
         <v>118</v>
       </c>
     </row>
@@ -4663,15 +4905,15 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+      <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4708,8 +4950,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4746,8 +4991,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -4782,6 +5030,9 @@
         <v>126</v>
       </c>
       <c r="L3" t="s">
+        <v>126</v>
+      </c>
+      <c r="M3" t="s">
         <v>126</v>
       </c>
     </row>
@@ -4793,15 +5044,15 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9B0605-DB41-5741-AA2A-D1CA2C98BE32}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:L3"/>
+      <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4838,8 +5089,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -4876,8 +5130,11 @@
       <c r="L2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -4912,6 +5169,9 @@
         <v>21</v>
       </c>
       <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -4923,15 +5183,15 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0B3097-2DFA-944C-921C-4CA3796F226E}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4968,8 +5228,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -5006,8 +5269,11 @@
       <c r="L2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -5044,8 +5310,11 @@
       <c r="L3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -5080,6 +5349,9 @@
         <v>21</v>
       </c>
       <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -5094,15 +5366,15 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5139,8 +5411,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5175,6 +5450,9 @@
         <v>21</v>
       </c>
       <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -5185,15 +5463,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D958EF-8599-434E-A913-0F7C0F849184}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="L2" sqref="L2:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5230,8 +5508,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5268,8 +5549,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -5306,8 +5590,11 @@
       <c r="L3" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -5344,8 +5631,11 @@
       <c r="L4" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>143</v>
       </c>
@@ -5382,8 +5672,11 @@
       <c r="L5" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -5402,8 +5695,11 @@
       <c r="L6" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -5440,8 +5736,11 @@
       <c r="L7" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -5478,8 +5777,11 @@
       <c r="L8" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>146</v>
       </c>
@@ -5514,6 +5816,9 @@
         <v>153</v>
       </c>
       <c r="L9" t="s">
+        <v>153</v>
+      </c>
+      <c r="M9" t="s">
         <v>153</v>
       </c>
     </row>
@@ -5525,15 +5830,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0776E127-336D-024E-B80F-189404F591FC}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:L6"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5570,8 +5875,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5608,8 +5916,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -5646,8 +5957,11 @@
       <c r="L3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -5684,8 +5998,11 @@
       <c r="L4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -5722,8 +6039,11 @@
       <c r="L5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -5758,6 +6078,9 @@
         <v>56</v>
       </c>
       <c r="L6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" t="s">
         <v>56</v>
       </c>
     </row>
@@ -5768,15 +6091,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D59C18B-BA52-C041-ABFD-C422450B1893}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="B5:D5"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5813,8 +6136,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5851,8 +6177,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -5889,8 +6218,11 @@
       <c r="L3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -5927,8 +6259,11 @@
       <c r="L4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -5954,7 +6289,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -5992,7 +6327,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -6029,8 +6364,11 @@
       <c r="L7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -6067,8 +6405,11 @@
       <c r="L8" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -6106,7 +6447,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -6142,6 +6483,9 @@
       </c>
       <c r="L10" t="s">
         <v>72</v>
+      </c>
+      <c r="M10" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -6152,15 +6496,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436CD732-077E-A245-BAB2-7F1C7EC5ED29}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="M2" sqref="M2:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6197,8 +6541,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6235,8 +6582,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -6273,8 +6623,11 @@
       <c r="L3" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -6311,8 +6664,11 @@
       <c r="L4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -6349,8 +6705,11 @@
       <c r="L5" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -6385,7 +6744,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -6422,8 +6781,11 @@
       <c r="L7" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -6460,8 +6822,11 @@
       <c r="L8" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -6498,8 +6863,11 @@
       <c r="L9" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -6541,15 +6909,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE071F5-4AF3-934C-BA73-B5E93C1FEEBC}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6586,8 +6954,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6622,6 +6993,9 @@
         <v>21</v>
       </c>
       <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -6632,15 +7006,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE3D9D0-9815-524A-8D84-2AA7877C22EB}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6677,8 +7051,11 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6715,8 +7092,11 @@
       <c r="L2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -6753,8 +7133,11 @@
       <c r="L3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -6791,8 +7174,11 @@
       <c r="L4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -6829,8 +7215,11 @@
       <c r="L5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -6867,8 +7256,11 @@
       <c r="L6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -6905,8 +7297,11 @@
       <c r="L7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -6941,7 +7336,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -6978,8 +7373,11 @@
       <c r="L9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>211</v>
       </c>
@@ -7014,8 +7412,9 @@
         <v>226</v>
       </c>
       <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -7052,8 +7451,11 @@
       <c r="L11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -7090,8 +7492,11 @@
       <c r="L12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -7128,8 +7533,11 @@
       <c r="L13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -7166,8 +7574,11 @@
       <c r="L14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -7204,8 +7615,11 @@
       <c r="L15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>209</v>
       </c>
@@ -7242,8 +7656,11 @@
       <c r="L16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>208</v>
       </c>
@@ -7262,8 +7679,9 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
@@ -7298,6 +7716,9 @@
         <v>36</v>
       </c>
       <c r="L18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M18" s="4" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added period_interview to variable list, updated survival analysis for mortality
</commit_message>
<xml_diff>
--- a/data/CKM Variable List.xlsx
+++ b/data/CKM Variable List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishnasanaka/nhanes_ckm/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\nhanes_ckm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9E049D-D0FD-3844-BEFC-F447334C668D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D092AE32-9D8E-4314-AA48-9CBB559D5758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="4100" windowWidth="28800" windowHeight="15780" firstSheet="3" activeTab="9" xr2:uid="{9B035D0F-8A45-D344-8416-9889809E00CA}"/>
+    <workbookView xWindow="-16320" yWindow="-14520" windowWidth="16440" windowHeight="28440" firstSheet="7" activeTab="8" xr2:uid="{9B035D0F-8A45-D344-8416-9889809E00CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="26" r:id="rId1"/>
@@ -327,7 +327,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="259">
   <si>
     <t>variable</t>
   </si>
@@ -1098,6 +1098,12 @@
   </si>
   <si>
     <t>DIQ175A</t>
+  </si>
+  <si>
+    <t>interview_period</t>
+  </si>
+  <si>
+    <t>RIDEXMON</t>
   </si>
 </sst>
 </file>
@@ -1152,6 +1158,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1638,17 +1645,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -1659,7 +1666,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -1670,12 +1677,12 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="C4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="C5" t="s">
         <v>219</v>
       </c>
@@ -1689,13 +1696,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6929FDCF-EFFB-654F-B597-6A4AD8F87EA2}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1736,7 +1743,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1777,7 +1784,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1818,7 +1825,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1859,7 +1866,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1894,7 +1901,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -1935,7 +1942,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -1976,7 +1983,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -2017,7 +2024,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>85</v>
       </c>
@@ -2058,7 +2065,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -2084,7 +2091,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>255</v>
       </c>
@@ -2105,9 +2112,9 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2148,7 +2155,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2189,7 +2196,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>233</v>
       </c>
@@ -2230,7 +2237,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>226</v>
       </c>
@@ -2271,7 +2278,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>234</v>
       </c>
@@ -2325,12 +2332,12 @@
       <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2371,7 +2378,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2412,7 +2419,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>221</v>
       </c>
@@ -2453,7 +2460,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2479,9 +2486,9 @@
       <selection activeCell="L2" sqref="L2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2522,7 +2529,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2563,7 +2570,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -2618,9 +2625,9 @@
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2661,7 +2668,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2702,7 +2709,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -2743,7 +2750,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>222</v>
       </c>
@@ -2798,9 +2805,9 @@
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2841,7 +2848,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2882,7 +2889,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2937,9 +2944,9 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2980,7 +2987,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3018,7 +3025,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3056,7 +3063,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>242</v>
       </c>
@@ -3094,7 +3101,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -3132,7 +3139,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>246</v>
       </c>
@@ -3186,9 +3193,9 @@
       <selection activeCell="L2" sqref="L2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3229,7 +3236,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3270,7 +3277,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -3325,9 +3332,9 @@
       <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3368,7 +3375,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3422,12 +3429,12 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:M2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3468,7 +3475,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3523,13 +3530,13 @@
       <selection pane="topRight" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3570,7 +3577,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3611,7 +3618,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -3652,7 +3659,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -3693,7 +3700,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -3734,12 +3741,12 @@
       <selection activeCell="L2" sqref="L2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3780,7 +3787,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3821,7 +3828,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -3876,9 +3883,9 @@
       <selection activeCell="L2" sqref="L2:M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3919,7 +3926,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3960,7 +3967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -4001,7 +4008,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -4052,9 +4059,9 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4095,7 +4102,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4136,7 +4143,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -4174,7 +4181,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -4215,7 +4222,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -4253,7 +4260,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -4294,7 +4301,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -4332,7 +4339,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -4373,7 +4380,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -4411,7 +4418,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -4455,7 +4462,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>103</v>
       </c>
@@ -4493,7 +4500,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>104</v>
       </c>
@@ -4534,7 +4541,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>105</v>
       </c>
@@ -4585,9 +4592,9 @@
       <selection activeCell="J2" sqref="J2:M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4628,7 +4635,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4669,7 +4676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>203</v>
       </c>
@@ -4701,7 +4708,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>200</v>
       </c>
@@ -4733,7 +4740,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>201</v>
       </c>
@@ -4762,7 +4769,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="Q11" t="s">
         <v>173</v>
       </c>
@@ -4783,9 +4790,9 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4826,7 +4833,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4867,7 +4874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -4908,7 +4915,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -4962,9 +4969,9 @@
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5005,7 +5012,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5046,7 +5053,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -5087,7 +5094,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -5125,7 +5132,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -5179,9 +5186,9 @@
       <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5222,7 +5229,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5263,7 +5270,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -5320,9 +5327,9 @@
       <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5363,7 +5370,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5404,7 +5411,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -5459,9 +5466,9 @@
       <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5502,7 +5509,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -5543,7 +5550,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -5598,9 +5605,9 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5641,7 +5648,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -5682,7 +5689,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -5723,7 +5730,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -5781,9 +5788,9 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5824,7 +5831,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5878,9 +5885,9 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5921,7 +5928,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5962,7 +5969,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -6003,7 +6010,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -6044,7 +6051,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>143</v>
       </c>
@@ -6085,7 +6092,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -6108,7 +6115,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -6149,7 +6156,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -6190,7 +6197,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>146</v>
       </c>
@@ -6231,7 +6238,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>237</v>
       </c>
@@ -6283,9 +6290,9 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6326,7 +6333,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6367,7 +6374,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -6408,7 +6415,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -6449,7 +6456,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -6490,7 +6497,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -6544,9 +6551,9 @@
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6587,7 +6594,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6628,7 +6635,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -6669,7 +6676,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -6710,7 +6717,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -6736,7 +6743,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -6774,7 +6781,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -6815,7 +6822,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -6856,7 +6863,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -6894,7 +6901,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -6949,9 +6956,9 @@
       <selection activeCell="M2" sqref="M2:M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6992,7 +6999,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -7033,7 +7040,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -7074,7 +7081,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -7115,7 +7122,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -7156,7 +7163,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -7191,7 +7198,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -7232,7 +7239,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -7273,7 +7280,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -7314,7 +7321,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -7362,9 +7369,9 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7405,7 +7412,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -7453,15 +7460,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE3D9D0-9815-524A-8D84-2AA7877C22EB}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7502,7 +7509,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -7543,7 +7550,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -7584,588 +7591,629 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D4" t="s">
+        <v>258</v>
+      </c>
+      <c r="E4" t="s">
+        <v>258</v>
+      </c>
+      <c r="F4" t="s">
+        <v>258</v>
+      </c>
+      <c r="G4" t="s">
+        <v>258</v>
+      </c>
+      <c r="H4" t="s">
+        <v>258</v>
+      </c>
+      <c r="I4" t="s">
+        <v>258</v>
+      </c>
+      <c r="J4" t="s">
+        <v>258</v>
+      </c>
+      <c r="K4" t="s">
+        <v>258</v>
+      </c>
+      <c r="L4" t="s">
+        <v>258</v>
+      </c>
+      <c r="M4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G5" t="s">
         <v>24</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J5" t="s">
         <v>24</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K5" t="s">
         <v>24</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L5" t="s">
         <v>24</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
         <v>25</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" t="s">
         <v>42</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I6" t="s">
         <v>42</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J6" t="s">
         <v>42</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K6" t="s">
         <v>42</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L6" t="s">
         <v>42</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>36</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>36</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>36</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>36</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>36</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I7" t="s">
         <v>36</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J7" t="s">
         <v>36</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K7" t="s">
         <v>36</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L7" t="s">
         <v>36</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>192</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>192</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>192</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>192</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>190</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>190</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
         <v>26</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I8" t="s">
         <v>26</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J8" t="s">
         <v>26</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K8" t="s">
         <v>26</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L8" t="s">
         <v>26</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>37</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>38</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>38</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>38</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>38</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I9" t="s">
         <v>38</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J9" t="s">
         <v>38</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>28</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>28</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>28</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I10" t="s">
         <v>28</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J10" t="s">
         <v>28</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K10" t="s">
         <v>28</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L10" t="s">
         <v>28</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A11" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K11" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>41</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>41</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>41</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>41</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H12" t="s">
         <v>41</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I12" t="s">
         <v>41</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J12" t="s">
         <v>41</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>41</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L12" t="s">
         <v>29</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>30</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>30</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>30</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>30</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>30</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I13" t="s">
         <v>30</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J13" t="s">
         <v>30</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K13" t="s">
         <v>30</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L13" t="s">
         <v>30</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>31</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>31</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>31</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>31</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" t="s">
         <v>31</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H14" t="s">
         <v>31</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I14" t="s">
         <v>31</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J14" t="s">
         <v>31</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K14" t="s">
         <v>31</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L14" t="s">
         <v>31</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>32</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>32</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>32</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H15" t="s">
         <v>32</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I15" t="s">
         <v>32</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J15" t="s">
         <v>32</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K15" t="s">
         <v>32</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L15" t="s">
         <v>32</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>39</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>39</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>39</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>39</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>39</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>39</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H16" t="s">
         <v>39</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I16" t="s">
         <v>39</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J16" t="s">
         <v>39</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K16" t="s">
         <v>39</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L16" t="s">
         <v>33</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>207</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>40</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>40</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>40</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>40</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>40</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>40</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H17" t="s">
         <v>40</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I17" t="s">
         <v>40</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J17" t="s">
         <v>40</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K17" t="s">
         <v>40</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L17" t="s">
         <v>34</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A18" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="L19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="M19" s="4" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added fasting insulin level comment
</commit_message>
<xml_diff>
--- a/data/CKM Variable List.xlsx
+++ b/data/CKM Variable List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\nhanes_ckm\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishnasanaka/nhanes_ckm/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D092AE32-9D8E-4314-AA48-9CBB559D5758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696DC4E1-7AD6-F741-831D-E3B76F7F3162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-14520" windowWidth="16440" windowHeight="28440" firstSheet="7" activeTab="8" xr2:uid="{9B035D0F-8A45-D344-8416-9889809E00CA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" firstSheet="4" activeTab="19" xr2:uid="{9B035D0F-8A45-D344-8416-9889809E00CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="26" r:id="rId1"/>
@@ -283,7 +283,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    uU/mL</t>
+    uU/mL
+Reply:
+    Fasting insulin</t>
       </text>
     </comment>
   </commentList>
@@ -1618,6 +1620,9 @@
   <threadedComment ref="A3" dT="2024-08-01T15:54:55.24" personId="{633F7228-773A-9346-9C6F-7677A288705B}" id="{982B6A64-B4D9-564C-AFD6-AA3C75D92EAD}">
     <text>uU/mL</text>
   </threadedComment>
+  <threadedComment ref="A3" dT="2025-02-19T22:44:42.22" personId="{633F7228-773A-9346-9C6F-7677A288705B}" id="{99E63FF9-A67B-D143-B6BB-4638362DF2BD}" parentId="{982B6A64-B4D9-564C-AFD6-AA3C75D92EAD}">
+    <text>Fasting insulin</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1645,17 +1650,17 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>214</v>
       </c>
@@ -1666,7 +1671,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>212</v>
       </c>
@@ -1677,12 +1682,12 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>219</v>
       </c>
@@ -1697,12 +1702,12 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1743,7 +1748,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1784,7 +1789,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1825,7 +1830,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1866,7 +1871,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1901,7 +1906,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -1942,7 +1947,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -1983,7 +1988,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -2024,7 +2029,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>85</v>
       </c>
@@ -2065,7 +2070,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -2091,7 +2096,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>255</v>
       </c>
@@ -2112,9 +2117,9 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2155,7 +2160,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2196,7 +2201,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>233</v>
       </c>
@@ -2237,7 +2242,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>226</v>
       </c>
@@ -2278,7 +2283,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>234</v>
       </c>
@@ -2332,12 +2337,12 @@
       <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2378,7 +2383,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2419,7 +2424,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>221</v>
       </c>
@@ -2460,7 +2465,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2486,9 +2491,9 @@
       <selection activeCell="L2" sqref="L2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2529,7 +2534,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2570,7 +2575,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -2622,12 +2627,12 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2668,7 +2673,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2709,7 +2714,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -2750,7 +2755,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>222</v>
       </c>
@@ -2805,9 +2810,9 @@
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2848,7 +2853,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2889,7 +2894,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -2944,9 +2949,9 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2987,7 +2992,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3025,7 +3030,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>240</v>
       </c>
@@ -3063,7 +3068,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>242</v>
       </c>
@@ -3101,7 +3106,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -3139,7 +3144,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>246</v>
       </c>
@@ -3193,9 +3198,9 @@
       <selection activeCell="L2" sqref="L2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3236,7 +3241,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3277,7 +3282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -3332,9 +3337,9 @@
       <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3375,7 +3380,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3432,9 +3437,9 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3475,7 +3480,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3530,13 +3535,13 @@
       <selection pane="topRight" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3577,7 +3582,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3618,7 +3623,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>119</v>
       </c>
@@ -3659,7 +3664,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -3700,7 +3705,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -3737,16 +3742,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F8F56B-9E15-EF47-B5F6-D90A8D8B0453}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3787,7 +3792,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3828,7 +3833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -3883,9 +3888,9 @@
       <selection activeCell="L2" sqref="L2:M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3926,7 +3931,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3967,7 +3972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -4008,7 +4013,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -4059,9 +4064,9 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4102,7 +4107,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4143,7 +4148,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -4181,7 +4186,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>96</v>
       </c>
@@ -4222,7 +4227,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>97</v>
       </c>
@@ -4260,7 +4265,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>98</v>
       </c>
@@ -4301,7 +4306,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -4339,7 +4344,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>100</v>
       </c>
@@ -4380,7 +4385,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -4418,7 +4423,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -4462,7 +4467,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>103</v>
       </c>
@@ -4500,7 +4505,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>104</v>
       </c>
@@ -4541,7 +4546,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>105</v>
       </c>
@@ -4592,9 +4597,9 @@
       <selection activeCell="J2" sqref="J2:M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4635,7 +4640,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4676,7 +4681,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>203</v>
       </c>
@@ -4708,7 +4713,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>200</v>
       </c>
@@ -4740,7 +4745,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>201</v>
       </c>
@@ -4769,7 +4774,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="Q11" t="s">
         <v>173</v>
       </c>
@@ -4790,9 +4795,9 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4833,7 +4838,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4874,7 +4879,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>107</v>
       </c>
@@ -4915,7 +4920,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -4969,9 +4974,9 @@
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5012,7 +5017,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5053,7 +5058,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -5094,7 +5099,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -5132,7 +5137,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -5186,9 +5191,9 @@
       <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5229,7 +5234,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5270,7 +5275,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -5327,9 +5332,9 @@
       <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5370,7 +5375,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5411,7 +5416,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>125</v>
       </c>
@@ -5466,9 +5471,9 @@
       <selection activeCell="M2" sqref="M2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5509,7 +5514,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>131</v>
       </c>
@@ -5550,7 +5555,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -5605,9 +5610,9 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5648,7 +5653,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -5689,7 +5694,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -5730,7 +5735,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -5788,9 +5793,9 @@
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5831,7 +5836,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5885,9 +5890,9 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5928,7 +5933,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5969,7 +5974,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -6010,7 +6015,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -6051,7 +6056,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>143</v>
       </c>
@@ -6092,7 +6097,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -6115,7 +6120,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -6156,7 +6161,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -6197,7 +6202,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>146</v>
       </c>
@@ -6238,7 +6243,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>237</v>
       </c>
@@ -6290,9 +6295,9 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6333,7 +6338,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6374,7 +6379,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -6415,7 +6420,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -6456,7 +6461,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -6497,7 +6502,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -6551,9 +6556,9 @@
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6594,7 +6599,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6635,7 +6640,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -6676,7 +6681,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -6717,7 +6722,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -6743,7 +6748,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -6781,7 +6786,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>65</v>
       </c>
@@ -6822,7 +6827,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -6863,7 +6868,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -6901,7 +6906,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -6956,9 +6961,9 @@
       <selection activeCell="M2" sqref="M2:M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6999,7 +7004,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -7040,7 +7045,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -7081,7 +7086,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -7122,7 +7127,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -7163,7 +7168,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -7198,7 +7203,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -7239,7 +7244,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -7280,7 +7285,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -7321,7 +7326,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -7369,9 +7374,9 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7412,7 +7417,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -7462,13 +7467,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE3D9D0-9815-524A-8D84-2AA7877C22EB}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7509,7 +7514,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -7550,7 +7555,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -7591,7 +7596,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>257</v>
       </c>
@@ -7632,7 +7637,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -7673,7 +7678,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -7714,7 +7719,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -7755,7 +7760,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -7796,7 +7801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -7831,7 +7836,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -7872,7 +7877,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>209</v>
       </c>
@@ -7909,7 +7914,7 @@
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -7950,7 +7955,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -7991,7 +7996,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -8032,7 +8037,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -8073,7 +8078,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -8114,7 +8119,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>207</v>
       </c>
@@ -8155,7 +8160,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>206</v>
       </c>
@@ -8176,7 +8181,7 @@
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Updated for instructional video
</commit_message>
<xml_diff>
--- a/data/CKM Variable List.xlsx
+++ b/data/CKM Variable List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\nhanes_ckm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C4E584-6031-4655-B442-BFA536060B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADE9ADD-0715-42E0-AB8B-467DDF70C887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-13110" windowWidth="38620" windowHeight="21220" xr2:uid="{9B035D0F-8A45-D344-8416-9889809E00CA}"/>
+    <workbookView xWindow="28680" yWindow="-3300" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{9B035D0F-8A45-D344-8416-9889809E00CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="26" r:id="rId1"/>
@@ -327,7 +327,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="261">
   <si>
     <t>variable</t>
   </si>
@@ -1104,6 +1104,12 @@
   </si>
   <si>
     <t>RIDEXMON</t>
+  </si>
+  <si>
+    <t>armcircumference</t>
+  </si>
+  <si>
+    <t>BMXARMC</t>
   </si>
 </sst>
 </file>
@@ -1641,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57554723-4699-4F6C-909F-85B73BE17680}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -6284,10 +6290,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0776E127-336D-024E-B80F-189404F591FC}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -6536,6 +6542,47 @@
       </c>
       <c r="M6" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>259</v>
+      </c>
+      <c r="B7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" t="s">
+        <v>260</v>
+      </c>
+      <c r="D7" t="s">
+        <v>260</v>
+      </c>
+      <c r="E7" t="s">
+        <v>260</v>
+      </c>
+      <c r="F7" t="s">
+        <v>260</v>
+      </c>
+      <c r="G7" t="s">
+        <v>260</v>
+      </c>
+      <c r="H7" t="s">
+        <v>260</v>
+      </c>
+      <c r="I7" t="s">
+        <v>260</v>
+      </c>
+      <c r="J7" t="s">
+        <v>260</v>
+      </c>
+      <c r="K7" t="s">
+        <v>260</v>
+      </c>
+      <c r="L7" t="s">
+        <v>260</v>
+      </c>
+      <c r="M7" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added variables of Visceral adipose tissue mass and Subcutaneous fat mass for 2011-2018.
</commit_message>
<xml_diff>
--- a/data/CKM Variable List.xlsx
+++ b/data/CKM Variable List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\external\nhanes_ckm\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JGUO258\Documents\JGUO\papers repo\nhanes_ckm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADE9ADD-0715-42E0-AB8B-467DDF70C887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEC2C4F-CB66-4AAC-8DB6-1B5B1F7DD020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3300" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{9B035D0F-8A45-D344-8416-9889809E00CA}"/>
+    <workbookView xWindow="-25320" yWindow="240" windowWidth="25440" windowHeight="15390" activeTab="11" xr2:uid="{9B035D0F-8A45-D344-8416-9889809E00CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="26" r:id="rId1"/>
@@ -24,24 +24,25 @@
     <sheet name="DEMO" sheetId="8" r:id="rId9"/>
     <sheet name="DIQ" sheetId="9" r:id="rId10"/>
     <sheet name="DXX" sheetId="30" r:id="rId11"/>
-    <sheet name="FASTQX" sheetId="27" r:id="rId12"/>
-    <sheet name="GHB" sheetId="10" r:id="rId13"/>
-    <sheet name="GLU" sheetId="11" r:id="rId14"/>
-    <sheet name="HDL" sheetId="12" r:id="rId15"/>
-    <sheet name="HIQ" sheetId="31" r:id="rId16"/>
-    <sheet name="HSCRP" sheetId="13" r:id="rId17"/>
-    <sheet name="HUQ" sheetId="14" r:id="rId18"/>
-    <sheet name="INQ" sheetId="15" r:id="rId19"/>
-    <sheet name="INS" sheetId="16" r:id="rId20"/>
-    <sheet name="KIQ_U" sheetId="17" r:id="rId21"/>
-    <sheet name="MCQ" sheetId="18" r:id="rId22"/>
-    <sheet name="OGTT" sheetId="25" r:id="rId23"/>
-    <sheet name="RXQASA" sheetId="19" r:id="rId24"/>
-    <sheet name="SMQ" sheetId="20" r:id="rId25"/>
-    <sheet name="SMQRTU" sheetId="21" r:id="rId26"/>
-    <sheet name="SSAGP" sheetId="22" r:id="rId27"/>
-    <sheet name="TCHOL" sheetId="23" r:id="rId28"/>
-    <sheet name="TRIGLY" sheetId="24" r:id="rId29"/>
+    <sheet name="DXXAG" sheetId="32" r:id="rId12"/>
+    <sheet name="FASTQX" sheetId="27" r:id="rId13"/>
+    <sheet name="GHB" sheetId="10" r:id="rId14"/>
+    <sheet name="GLU" sheetId="11" r:id="rId15"/>
+    <sheet name="HDL" sheetId="12" r:id="rId16"/>
+    <sheet name="HIQ" sheetId="31" r:id="rId17"/>
+    <sheet name="HSCRP" sheetId="13" r:id="rId18"/>
+    <sheet name="HUQ" sheetId="14" r:id="rId19"/>
+    <sheet name="INQ" sheetId="15" r:id="rId20"/>
+    <sheet name="INS" sheetId="16" r:id="rId21"/>
+    <sheet name="KIQ_U" sheetId="17" r:id="rId22"/>
+    <sheet name="MCQ" sheetId="18" r:id="rId23"/>
+    <sheet name="OGTT" sheetId="25" r:id="rId24"/>
+    <sheet name="RXQASA" sheetId="19" r:id="rId25"/>
+    <sheet name="SMQ" sheetId="20" r:id="rId26"/>
+    <sheet name="SMQRTU" sheetId="21" r:id="rId27"/>
+    <sheet name="SSAGP" sheetId="22" r:id="rId28"/>
+    <sheet name="TCHOL" sheetId="23" r:id="rId29"/>
+    <sheet name="TRIGLY" sheetId="24" r:id="rId30"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -327,7 +328,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1934" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1970" uniqueCount="265">
   <si>
     <t>variable</t>
   </si>
@@ -1110,6 +1111,18 @@
   </si>
   <si>
     <t>BMXARMC</t>
+  </si>
+  <si>
+    <t>visceral_fat</t>
+  </si>
+  <si>
+    <t>subcutaneous_fat</t>
+  </si>
+  <si>
+    <t>DXXVFATM</t>
+  </si>
+  <si>
+    <t>DXXSATM</t>
   </si>
 </sst>
 </file>
@@ -2115,7 +2128,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -2331,6 +2344,137 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885DB13C-D9BF-4173-81AE-B0DAA0BC51F0}">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>262</v>
+      </c>
+      <c r="H3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I3" t="s">
+        <v>264</v>
+      </c>
+      <c r="J3" t="s">
+        <v>264</v>
+      </c>
+      <c r="K3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>261</v>
+      </c>
+      <c r="H4" t="s">
+        <v>263</v>
+      </c>
+      <c r="I4" t="s">
+        <v>263</v>
+      </c>
+      <c r="J4" t="s">
+        <v>263</v>
+      </c>
+      <c r="K4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B87265F-26C7-4386-8B52-059591A00490}">
   <dimension ref="A1:M4"/>
   <sheetViews>
@@ -2484,7 +2628,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C29EFAD-03F0-B447-A983-4B5565025BC2}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -2623,7 +2767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{270977A7-E7B7-C047-9DBF-59746F13B1CD}">
   <dimension ref="A1:M4"/>
   <sheetViews>
@@ -2803,7 +2947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85252202-D3B5-A945-8429-01698367E2C9}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -2942,7 +3086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E249D9-7D36-2A4C-8D0E-BDBA5CAA1DE0}">
   <dimension ref="A1:M6"/>
   <sheetViews>
@@ -3188,7 +3332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C686534B-BF02-8740-9CD8-A73AF60469ED}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -3330,112 +3474,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC757E38-DF6E-9C47-986A-E5D523B85FF9}">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:M2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A8F896-8412-FD4D-A653-D930D501E3F0}">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="A1:M2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -3740,6 +3784,106 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A8F896-8412-FD4D-A653-D930D501E3F0}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37F8F56B-9E15-EF47-B5F6-D90A8D8B0453}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -3881,7 +4025,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B22359-510C-BD4E-946F-DF74FC3CE91E}">
   <dimension ref="A1:M4"/>
   <sheetViews>
@@ -4057,7 +4201,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C695FBCA-2F20-C349-9C97-E127EC92AD35}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
@@ -4590,7 +4734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B443EBC9-A9ED-4996-AA7B-B560C4AE0236}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
@@ -4785,7 +4929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98AD27C-16C2-BE4F-BECC-445339C348A0}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -4967,7 +5111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF0C966-3BAC-4E46-A712-3678781F85CE}">
   <dimension ref="A1:M5"/>
   <sheetViews>
@@ -5184,7 +5328,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40400EB-A076-D749-9395-73DB4F782CEE}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -5322,7 +5466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1A5F4B-3A4F-C646-B6D8-2975540D552C}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -5464,7 +5608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9B0605-DB41-5741-AA2A-D1CA2C98BE32}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -5594,186 +5738,6 @@
         <v>21</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0B3097-2DFA-944C-921C-4CA3796F226E}">
-  <dimension ref="A1:M4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F2" t="s">
-        <v>188</v>
-      </c>
-      <c r="G2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I2" t="s">
-        <v>188</v>
-      </c>
-      <c r="J2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K2" t="s">
-        <v>161</v>
-      </c>
-      <c r="L2" t="s">
-        <v>161</v>
-      </c>
-      <c r="M2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I3" t="s">
-        <v>130</v>
-      </c>
-      <c r="J3" t="s">
-        <v>130</v>
-      </c>
-      <c r="K3" t="s">
-        <v>130</v>
-      </c>
-      <c r="L3" t="s">
-        <v>130</v>
-      </c>
-      <c r="M3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -5883,6 +5847,186 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD0B3097-2DFA-944C-921C-4CA3796F226E}">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G2" t="s">
+        <v>188</v>
+      </c>
+      <c r="H2" t="s">
+        <v>188</v>
+      </c>
+      <c r="I2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J2" t="s">
+        <v>188</v>
+      </c>
+      <c r="K2" t="s">
+        <v>161</v>
+      </c>
+      <c r="L2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" t="s">
+        <v>130</v>
+      </c>
+      <c r="K3" t="s">
+        <v>130</v>
+      </c>
+      <c r="L3" t="s">
+        <v>130</v>
+      </c>
+      <c r="M3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D958EF-8599-434E-A913-0F7C0F849184}">
   <dimension ref="A1:M10"/>
@@ -6292,7 +6436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0776E127-336D-024E-B80F-189404F591FC}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -7509,7 +7653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE3D9D0-9815-524A-8D84-2AA7877C22EB}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>

</xml_diff>